<commit_message>
Refactored rook's GetMovesFrom ; Added Bishop class
</commit_message>
<xml_diff>
--- a/Working.xlsx
+++ b/Working.xlsx
@@ -16,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Things I don't like</t>
   </si>
   <si>
-    <t>CodeRush issues</t>
-  </si>
-  <si>
-    <t>Board takes "pawn" as an argument instead of "piece"</t>
-  </si>
-  <si>
-    <t>Classes are inline in test classes</t>
-  </si>
-  <si>
     <t>Production code not in its own project</t>
   </si>
   <si>
@@ -39,19 +30,34 @@
     <t>Pawn doesn't have diagonal capture capability</t>
   </si>
   <si>
-    <t>Rook's constructor test is kind of stupid</t>
-  </si>
-  <si>
-    <t>Rook's GetMovesFrom is very stupid</t>
-  </si>
-  <si>
-    <t>Pawn should get two moves for its first move</t>
-  </si>
-  <si>
     <t>…but I'll worry about later</t>
   </si>
   <si>
     <t>We need to figure out how "HasMoved" gets set</t>
+  </si>
+  <si>
+    <t>I wish Rook.GetMovesFrom were more Linq-y</t>
+  </si>
+  <si>
+    <t>We've got Rook, so why not Bishop</t>
+  </si>
+  <si>
+    <t>And queen?</t>
+  </si>
+  <si>
+    <t>And king?</t>
+  </si>
+  <si>
+    <t>And maybe knight</t>
+  </si>
+  <si>
+    <t>I'm going to have the same default board size in a lot of tests</t>
+  </si>
+  <si>
+    <t>At some point, additional tests on bishop.GetMovesFrom</t>
+  </si>
+  <si>
+    <t>Refactor ugly Bishop.GetMovesFrom</t>
   </si>
 </sst>
 </file>
@@ -422,12 +428,12 @@
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -436,50 +442,58 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
+      <c r="A8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
+      <c r="A10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>